<commit_message>
new changes, rn implemented, after the scare
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -534,16 +534,16 @@
         <v>13</v>
       </c>
       <c r="B2" s="4">
-        <v>94.85</v>
+        <v>94.47</v>
       </c>
       <c r="C2" s="4">
-        <v>95.96</v>
+        <v>95.9</v>
       </c>
       <c r="D2" s="4">
-        <v>93.35</v>
+        <v>93.02</v>
       </c>
       <c r="E2" s="4">
-        <v>94.64</v>
+        <v>94.63</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>

</xml_diff>

<commit_message>
new changes, update pca
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -534,16 +534,16 @@
         <v>13</v>
       </c>
       <c r="B2" s="4">
-        <v>94.47</v>
+        <v>94.66</v>
       </c>
       <c r="C2" s="4">
         <v>95.9</v>
       </c>
       <c r="D2" s="4">
-        <v>93.02</v>
+        <v>93.01</v>
       </c>
       <c r="E2" s="4">
-        <v>94.63</v>
+        <v>94.62</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>

</xml_diff>